<commit_message>
commit for design milestone
</commit_message>
<xml_diff>
--- a/CRC Diagram-StockAdvisor.xlsx
+++ b/CRC Diagram-StockAdvisor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chenming\Documents\MCIT591\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/chenming_ualberta_ca/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6264106B-F528-46D9-BE95-AAB76A875BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{BE56F94C-7A01-4BC2-82F5-B76D88AF32E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF103B58-AF5A-40C8-BA15-3C8221940724}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="855" windowWidth="21600" windowHeight="11385" xr2:uid="{B5D6E086-E7E5-44B1-9ABE-77B1D2E8539C}"/>
+    <workbookView xWindow="5025" yWindow="465" windowWidth="21600" windowHeight="11385" xr2:uid="{B5D6E086-E7E5-44B1-9ABE-77B1D2E8539C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Responsibilities</t>
   </si>
@@ -49,21 +49,12 @@
   </si>
   <si>
     <t>YahooFinanceDataReader</t>
-  </si>
-  <si>
-    <t>ARIMAShortTermAnalysis</t>
-  </si>
-  <si>
-    <t>ARMALongTermAnalysis</t>
   </si>
   <si>
     <t>UserInput
 UserOutput</t>
   </si>
   <si>
-    <t>pullStockData</t>
-  </si>
-  <si>
     <t>DataProcessor</t>
   </si>
   <si>
@@ -71,27 +62,12 @@
   </si>
   <si>
     <t>runARMA</t>
-  </si>
-  <si>
-    <t>readStockTickerSymbol
-readDateRange
-readInvestmentHorizon</t>
-  </si>
-  <si>
-    <t>UserInput
-YahooFinanceDataReader
-ARIMAShortTermAnalysis
-ARMALongTermAnalysis
-UserOutput</t>
   </si>
   <si>
     <t>UserInterface
 YahooFinanceDataReader</t>
   </si>
   <si>
-    <t>dataProcessing</t>
-  </si>
-  <si>
     <t>dataVisualization
 giveRecommendation</t>
   </si>
@@ -102,16 +78,46 @@
     <t>runStockAdvisor</t>
   </si>
   <si>
+    <t>DataProcessor
+UserInterface</t>
+  </si>
+  <si>
     <t>createAndShowGUI
 askStockTickerSymbol
-askDateRange
 askInvestmentHorizon
 startDataProcessing
 showRecommendationResult</t>
   </si>
   <si>
-    <t>DataProcessor
-UserInterface</t>
+    <t>readStockTickerSymbol
+readInvestmentHorizon</t>
+  </si>
+  <si>
+    <t>UserInput
+DataProcessor</t>
+  </si>
+  <si>
+    <t>getStock
+generatePriceList
+getHistoricalPrices</t>
+  </si>
+  <si>
+    <t>calculateAverage
+dataProcessing
+getRecommendation</t>
+  </si>
+  <si>
+    <t>ARIMAAnalysis</t>
+  </si>
+  <si>
+    <t>ARMAAnalysis</t>
+  </si>
+  <si>
+    <t>UserInput
+YahooFinanceDataReader
+ARIMAAnalysis
+ARMAAnalysis
+UserOutput</t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,19 +580,19 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -617,12 +623,12 @@
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -648,31 +654,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="D11" s="4" t="s">
@@ -696,21 +702,21 @@
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5"/>
     </row>
@@ -724,7 +730,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>2</v>
@@ -732,15 +738,249 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D0B80CB4FB521A4C88D04172A3A6558C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2108635b6d752fef38fff34331cf89e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a93742a8-a1e4-45ad-9f5a-8d882bb07a21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ce89623fd6cfd54fa4234035ae649cc" ns3:_="">
+    <xsd:import namespace="a93742a8-a1e4-45ad-9f5a-8d882bb07a21"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a93742a8-a1e4-45ad-9f5a-8d882bb07a21" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{593145D9-E699-4BAB-BDC6-1C78F768FE59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a93742a8-a1e4-45ad-9f5a-8d882bb07a21"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D31BBB-660A-4C90-AB9F-356BDE1D6F9D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E03FCFB-D218-41CD-BF83-13445277E087}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>